<commit_message>
Adding script for graphs done for portfolio
</commit_message>
<xml_diff>
--- a/Sent to Client/Instacart Final Report.xlsx
+++ b/Sent to Client/Instacart Final Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisaa\Instacart Project\Sent to Client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc2fde4a95f98d49/Desktop/Instacart-Project/Sent to Client/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E7011C-C353-43E6-9AEE-4AB5948205C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="808" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="808" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Title Page" sheetId="1" r:id="rId1"/>
@@ -22054,7 +22054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="45.75" thickTop="1">
+    <row r="7" spans="2:9" ht="30.75" thickTop="1">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
@@ -23005,8 +23005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:Q186"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG186" sqref="AG186"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A177" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186:M186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>